<commit_message>
yhfuhad cashpayments test case push
</commit_message>
<xml_diff>
--- a/test_case/cash_payments/Functional Testing/Pagination & Per Page.xlsx
+++ b/test_case/cash_payments/Functional Testing/Pagination & Per Page.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PNT SQA\Project\ai-quizwhiz.zluck.com-pnt-b24\test_case\cash_payments\Functional Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3C68DD-CBC7-4751-8D3F-ABA4375B4436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2F5C32-4EC9-4350-943E-2F633E678AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagination &amp; Per Page Filter" sheetId="1" r:id="rId1"/>
@@ -1214,7 +1214,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>